<commit_message>
Updating Springbacklog.xlsx ,deleting redundant file
</commit_message>
<xml_diff>
--- a/Sprint Backlog .xlsx
+++ b/Sprint Backlog .xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Task ID</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>searchFlights.php</t>
+  </si>
+  <si>
+    <t>LoginAttempt.php</t>
+  </si>
+  <si>
+    <t>ListOfPassengersBE.php</t>
+  </si>
+  <si>
+    <t>ListOfFlightsBE.php</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1115,7 @@
   <dimension ref="D2:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,15 +1502,23 @@
     </row>
     <row r="14" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="7"/>
       <c r="K14" s="20"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="M14" s="5">
+        <v>3</v>
+      </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="11"/>
@@ -1514,13 +1531,21 @@
     </row>
     <row r="15" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="20"/>
+      <c r="K15" s="20">
+        <v>1</v>
+      </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
@@ -1535,13 +1560,21 @@
     </row>
     <row r="16" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="20"/>
+      <c r="K16" s="20">
+        <v>1</v>
+      </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>

</xml_diff>